<commit_message>
Added CodigoDistribuidor from master to output
</commit_message>
<xml_diff>
--- a/homologacion_results/matched_clorox_cleaned.xlsx
+++ b/homologacion_results/matched_clorox_cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="36">
   <si>
     <t>CODIGODISTRIBUIDOR</t>
   </si>
@@ -479,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -615,16 +615,16 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>14005952</v>
+        <v>11001791.3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5">
-        <v>58.33333333333333</v>
+        <v>62.74509803921568</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
@@ -647,16 +647,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>14006766</v>
+        <v>11001791.3</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6">
-        <v>55.31914893617022</v>
+        <v>62.74509803921568</v>
       </c>
       <c r="E6" t="s">
         <v>33</v>
@@ -671,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="s">
         <v>35</v>
@@ -679,16 +679,16 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>14005952</v>
+        <v>11001791.3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7">
-        <v>58.33333333333333</v>
+        <v>62.74509803921568</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
@@ -711,16 +711,16 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>11000273</v>
+        <v>11001791.3</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8">
-        <v>58.62068965517242</v>
+        <v>62.74509803921568</v>
       </c>
       <c r="E8" t="s">
         <v>33</v>
@@ -743,16 +743,16 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
-        <v>14001197</v>
+        <v>11001791.3</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9">
-        <v>62.22222222222222</v>
+        <v>62.74509803921568</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
@@ -767,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="s">
         <v>35</v>
@@ -775,16 +775,16 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>11002101</v>
+        <v>11001791.3</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D10">
-        <v>61.90476190476191</v>
+        <v>62.74509803921568</v>
       </c>
       <c r="E10" t="s">
         <v>33</v>
@@ -807,13 +807,16 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>11001846</v>
+        <v>11001791.3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D11">
-        <v>40</v>
+        <v>62.74509803921568</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
@@ -836,16 +839,16 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>11002670</v>
+        <v>11001791.3</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D12">
-        <v>45.71428571428572</v>
+        <v>62.74509803921568</v>
       </c>
       <c r="E12" t="s">
         <v>33</v>
@@ -868,16 +871,16 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>14006766</v>
+        <v>14005952</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D13">
-        <v>59.57446808510638</v>
+        <v>58.33333333333333</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -900,16 +903,16 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>14006766</v>
+        <v>14005952</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D14">
-        <v>72.72727272727273</v>
+        <v>58.33333333333333</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
@@ -932,33 +935,606 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>11000310</v>
+        <v>14005952</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
       </c>
       <c r="D15">
+        <v>58.33333333333333</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>14006766</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>55.31914893617022</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>14005952</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>58.33333333333333</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>14005952</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>58.33333333333333</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>14005952</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>58.33333333333333</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>11000273</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20">
+        <v>58.62068965517242</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>14001197</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21">
+        <v>62.22222222222222</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>11002101</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>61.90476190476191</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>11001846</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23">
+        <v>40</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>11002670</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24">
+        <v>45.71428571428572</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>14006766</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25">
+        <v>59.57446808510638</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>14006766</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26">
+        <v>59.57446808510638</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>14006766</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <v>72.72727272727273</v>
+      </c>
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>14006766</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28">
+        <v>72.72727272727273</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>14006766</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29">
+        <v>72.72727272727273</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>14006766</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30">
+        <v>72.72727272727273</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>11000310</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31">
         <v>62.5</v>
       </c>
-      <c r="E15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" t="b">
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" t="b">
         <v>1</v>
       </c>
-      <c r="I15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="I31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>11000310</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32">
+        <v>62.5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>11000310</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33">
+        <v>62.5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>